<commit_message>
1a: No standardization and no shuffle
</commit_message>
<xml_diff>
--- a/Task1a/Comparison_of_Methods.xlsx
+++ b/Task1a/Comparison_of_Methods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Git\Intro_to_ML\Task1a\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23467997-EBB9-49DF-8540-788968C5650A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B16F9DC-7673-4D1E-8D2F-A942085C48AD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{388136D5-05EE-48FB-9E3D-7AAA4631CB20}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Intro to ML</t>
   </si>
@@ -60,6 +60,10 @@
   <si>
     <t xml:space="preserve">Standardization of folds
 no intercept </t>
+  </si>
+  <si>
+    <t>No standardization
+shuffle when use kfold (seed = 1)</t>
   </si>
 </sst>
 </file>
@@ -425,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C0D8E8C-4147-432E-BB52-10B1B19B3A44}">
-  <dimension ref="B2:I10"/>
+  <dimension ref="B2:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,20 +444,21 @@
     <col min="6" max="6" width="29.6640625" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" customWidth="1"/>
     <col min="8" max="8" width="23.5546875" customWidth="1"/>
+    <col min="10" max="10" width="36.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
@@ -472,8 +477,11 @@
       <c r="H5" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>4.79651739253051</v>
       </c>
@@ -498,8 +506,11 @@
       <c r="I6" s="5">
         <v>4.9355260103810199</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J6" s="3">
+        <v>4.8006113476114498</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>4.7963482095920398</v>
       </c>
@@ -524,8 +535,11 @@
       <c r="I7" s="2">
         <v>5.0984501942275902</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J7" s="3">
+        <v>4.8002483703501797</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>4.8103033121673597</v>
       </c>
@@ -550,8 +564,11 @@
       <c r="I8" s="2">
         <v>5.2692225428146804</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J8" s="3">
+        <v>4.8127441256846701</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <v>4.8679920394007699</v>
       </c>
@@ -576,8 +593,11 @@
       <c r="I9" s="2">
         <v>4.9719385674310201</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J9" s="3">
+        <v>4.8634390971983104</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>4.9880593870815302</v>
       </c>
@@ -601,6 +621,9 @@
       </c>
       <c r="I10" s="2">
         <v>5.0732478071640603</v>
+      </c>
+      <c r="J10" s="3">
+        <v>4.9566232289732701</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
No standardization and no shuffle
</commit_message>
<xml_diff>
--- a/Task1a/Comparison_of_Methods.xlsx
+++ b/Task1a/Comparison_of_Methods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Git\Intro_to_ML\Task1a\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23467997-EBB9-49DF-8540-788968C5650A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B16F9DC-7673-4D1E-8D2F-A942085C48AD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{388136D5-05EE-48FB-9E3D-7AAA4631CB20}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Intro to ML</t>
   </si>
@@ -60,6 +60,10 @@
   <si>
     <t xml:space="preserve">Standardization of folds
 no intercept </t>
+  </si>
+  <si>
+    <t>No standardization
+shuffle when use kfold (seed = 1)</t>
   </si>
 </sst>
 </file>
@@ -425,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C0D8E8C-4147-432E-BB52-10B1B19B3A44}">
-  <dimension ref="B2:I10"/>
+  <dimension ref="B2:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,20 +444,21 @@
     <col min="6" max="6" width="29.6640625" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" customWidth="1"/>
     <col min="8" max="8" width="23.5546875" customWidth="1"/>
+    <col min="10" max="10" width="36.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:10" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
@@ -472,8 +477,11 @@
       <c r="H5" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>4.79651739253051</v>
       </c>
@@ -498,8 +506,11 @@
       <c r="I6" s="5">
         <v>4.9355260103810199</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J6" s="3">
+        <v>4.8006113476114498</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>4.7963482095920398</v>
       </c>
@@ -524,8 +535,11 @@
       <c r="I7" s="2">
         <v>5.0984501942275902</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J7" s="3">
+        <v>4.8002483703501797</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>4.8103033121673597</v>
       </c>
@@ -550,8 +564,11 @@
       <c r="I8" s="2">
         <v>5.2692225428146804</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J8" s="3">
+        <v>4.8127441256846701</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <v>4.8679920394007699</v>
       </c>
@@ -576,8 +593,11 @@
       <c r="I9" s="2">
         <v>4.9719385674310201</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J9" s="3">
+        <v>4.8634390971983104</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>4.9880593870815302</v>
       </c>
@@ -601,6 +621,9 @@
       </c>
       <c r="I10" s="2">
         <v>5.0732478071640603</v>
+      </c>
+      <c r="J10" s="3">
+        <v>4.9566232289732701</v>
       </c>
     </row>
   </sheetData>

</xml_diff>